<commit_message>
update descriptions of the datasets
</commit_message>
<xml_diff>
--- a/triadic_simulation/data/Triadic_Delegation_Dataset.xlsx
+++ b/triadic_simulation/data/Triadic_Delegation_Dataset.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\03 Projects\Master Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive\Desktop\Algorithm-Appreciation-and-Aversion-in-Triadic-Delegation-Settings\triadic_simulation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EF9500-5689-4466-B660-CB8C9F4674B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0EF054F-F63F-4E7E-8334-F558BC392512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="901" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="67185" yWindow="885" windowWidth="13140" windowHeight="13455" tabRatio="901" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="10" r:id="rId1"/>
@@ -641,8 +641,564 @@
     <t>Exogenous context</t>
   </si>
   <si>
+    <t>II. Data Structure</t>
+  </si>
+  <si>
+    <t>├── LEVEL 1 — Dynamic Panels (HMM Estimation &amp; Outcomes)</t>
+  </si>
+  <si>
+    <t>│   ├── panel_manager_period   [PRIMARY HMM ESTIMATION TABLE]</t>
+  </si>
+  <si>
+    <t>│   │      Purpose: Formal decision authority delegation &amp; learning dynamics</t>
+  </si>
+  <si>
+    <t>│   │   ├── Identifiers &amp; time index</t>
+  </si>
+  <si>
+    <t>│   │   │   ├── period_start_date</t>
+  </si>
+  <si>
+    <t>│   │   │   ├── period_end_date</t>
+  </si>
+  <si>
+    <t>│   │   │   ├── weeks_in_period</t>
+  </si>
+  <si>
+    <t>│   │   ├── Formal decision authority (HMM emissions)</t>
+  </si>
+  <si>
+    <t>│   │   │   ├── ai_decision_authority_share        [EMISSION 1]</t>
+  </si>
+  <si>
+    <t>│   │   │   └── mean_override_pct                   [EMISSION 2]</t>
+  </si>
+  <si>
+    <t>│   │   ├── Performance feedback (HMM transition drivers)</t>
+  </si>
+  <si>
+    <t>│   │   │   ├── kpi_operational_gap_index</t>
+  </si>
+  <si>
+    <t>│   │   │   ├── kpi_peer_pressure_index</t>
+  </si>
+  <si>
+    <t>│   │   │   └── bonus_eligibility_flag              [SALIENT SHOCK]</t>
+  </si>
+  <si>
+    <t>│   │   ├── Incentives &amp; governance context (controls / moderators)</t>
+  </si>
+  <si>
+    <t>│   │   ├── Environmental &amp; task context (controls)</t>
+  </si>
+  <si>
+    <t>│   │   │   ├── task_complexity_index</t>
+  </si>
+  <si>
+    <t>│   │   │   ├── supply_disruption_count</t>
+  </si>
+  <si>
+    <t>│   │   │   └── forecast_accuracy_mape</t>
+  </si>
+  <si>
+    <t>│   │   └── Derived lag variables (explicit)</t>
+  </si>
+  <si>
+    <t>│   │       ├── lag_ai_decision_authority_share</t>
+  </si>
+  <si>
+    <t>│   │       ├── lag_mean_override_pct</t>
+  </si>
+  <si>
+    <t>│   │       ├── lag_kpi_operational_gap_index</t>
+  </si>
+  <si>
+    <t>│   │       ├── lag_kpi_peer_pressure_index</t>
+  </si>
+  <si>
+    <t>│   │       ├── lag_bonus_eligibility_flag</t>
+  </si>
+  <si>
+    <t>│   │       └── lag_decision_latency_avg   (optional)</t>
+  </si>
+  <si>
+    <t>│   ├── panel_manager_period_outcomes   [POST-HMM VALIDATION / CONSEQUENCES]</t>
+  </si>
+  <si>
+    <t>│   │      Actor: Manager / Site</t>
+  </si>
+  <si>
+    <t>│   │      Purpose: Operational outcomes (not used for state identification)</t>
+  </si>
+  <si>
+    <t>│   │   ├── service_level_pct</t>
+  </si>
+  <si>
+    <t>│   │   ├── inventory_cost_eur</t>
+  </si>
+  <si>
+    <t>│   │   ├── expedite_cost_eur</t>
+  </si>
+  <si>
+    <t>│   │   ├── error_incident_count</t>
+  </si>
+  <si>
+    <t>│   │   └── production_disruption_minutes</t>
+  </si>
+  <si>
+    <t>│   └── panel_employee_period   [REAL AUTHORITY / EXECUTION PANEL]</t>
+  </si>
+  <si>
+    <t>│          Purpose: Execution responsibility &amp; coordination with AI</t>
+  </si>
+  <si>
+    <t>│       ├── Execution responsibility (real authority)</t>
+  </si>
+  <si>
+    <t>├── LEVEL 2 — Episode Data (Behavioral Micro-Foundations)</t>
+  </si>
+  <si>
+    <t>│   ├── decision_episode   [MANAGER ↔ AI MICRO-DECISIONS]</t>
+  </si>
+  <si>
+    <t>│   │      Purpose: Micro-level inputs aggregated into HMM emissions &amp; controls</t>
+  </si>
+  <si>
+    <t>│   │       ├── manager_action            (accept / partial / reject)</t>
+  </si>
+  <si>
+    <t>│   │       ├── override_pct              → mean_override_pct</t>
+  </si>
+  <si>
+    <t>│   │       └── time_to_decision           → decision_latency_avg</t>
+  </si>
+  <si>
+    <t>│   └── execution_episode   [EMPLOYEE ↔ AI MICRO-EXECUTION]</t>
+  </si>
+  <si>
+    <t>│          Purpose: Micro-level execution &amp; intervention behavior</t>
+  </si>
+  <si>
+    <t>└── LEVEL 3 — Master Data (Stable Attributes &amp; Context)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ├── manager_master   [HETEROGENEITY / MODERATION]</t>
+  </si>
+  <si>
+    <t>│   │   │   ├── kpi_industry_gap_index</t>
+  </si>
+  <si>
+    <t>period_start_date</t>
+  </si>
+  <si>
+    <t>Used for lag construction</t>
+  </si>
+  <si>
+    <t>period_end_date</t>
+  </si>
+  <si>
+    <t>—</t>
+  </si>
+  <si>
+    <t>weeks_in_period</t>
+  </si>
+  <si>
+    <t>Length of period</t>
+  </si>
+  <si>
+    <t>weeks</t>
+  </si>
+  <si>
+    <t>mean_override_pct</t>
+  </si>
+  <si>
+    <t>Average magnitude of manager overrides of AI recommendations</t>
+  </si>
+  <si>
+    <t>kpi_operational_gap_index</t>
+  </si>
+  <si>
+    <t>Composite index of within-team KPI change vs prior period</t>
+  </si>
+  <si>
+    <t>standardized index</t>
+  </si>
+  <si>
+    <t>kpi_peer_pressure_index</t>
+  </si>
+  <si>
+    <t>Composite index of KPI standing relative to peer teams</t>
+  </si>
+  <si>
+    <t>bonus_eligibility_flag</t>
+  </si>
+  <si>
+    <t>Salient incentive discontinuity</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>lag_ai_decision_authority_share</t>
+  </si>
+  <si>
+    <t>lag_mean_override_pct</t>
+  </si>
+  <si>
+    <t>lag_kpi_operational_gap_index</t>
+  </si>
+  <si>
+    <t>lag_kpi_peer_pressure_index</t>
+  </si>
+  <si>
+    <t>lag_bonus_eligibility_flag</t>
+  </si>
+  <si>
+    <t>IDENTIFIER</t>
+  </si>
+  <si>
+    <t>HMM_EMISSION</t>
+  </si>
+  <si>
+    <t>HMM_TRANSITION_DRIVER</t>
+  </si>
+  <si>
+    <t>HMM_TRANSITION_SHOCK</t>
+  </si>
+  <si>
+    <t>HMM_CONTROL</t>
+  </si>
+  <si>
+    <t>HMM_LAG</t>
+  </si>
+  <si>
+    <t>L1 panel (manager-period)</t>
+  </si>
+  <si>
+    <t>3-week decision period identifier</t>
+  </si>
+  <si>
+    <t>Shared across panel tables</t>
+  </si>
+  <si>
+    <t>Start date of the decision period</t>
+  </si>
+  <si>
+    <t>End date of the decision period</t>
+  </si>
+  <si>
+    <t>Typically 3</t>
+  </si>
+  <si>
+    <t>AI system version active during period</t>
+  </si>
+  <si>
+    <t>CONTEXT_MASTER</t>
+  </si>
+  <si>
+    <t>Share of decisions where manager delegates formal decision authority to AI</t>
+  </si>
+  <si>
+    <t>Primary state-identifying behavioral measure</t>
+  </si>
+  <si>
+    <t>Derived from decision_episode.override_pct</t>
+  </si>
+  <si>
+    <t>Reduced-form performance feedback signal</t>
+  </si>
+  <si>
+    <t>Captures peer comparison / relative pressure</t>
+  </si>
+  <si>
+    <t>Indicator that period performance affects bonus eligibility</t>
+  </si>
+  <si>
+    <t>Difficulty/tightness of targets assigned in period</t>
+  </si>
+  <si>
+    <t>Governance context; exogenous where possible</t>
+  </si>
+  <si>
+    <t>Emission/transition control (context difficulty)</t>
+  </si>
+  <si>
+    <t>Number of supply disruptions affecting manager scope in period</t>
+  </si>
+  <si>
+    <t>Exogenous operational turbulence</t>
+  </si>
+  <si>
+    <t>Forecast error (MAPE) for manager scope during period</t>
+  </si>
+  <si>
+    <t>Proxy for signal quality; lower is better</t>
+  </si>
+  <si>
+    <t>Lagged AI decision authority share (t−1)</t>
+  </si>
+  <si>
+    <t>Derived from prior period</t>
+  </si>
+  <si>
+    <t>Lagged override magnitude (t−1)</t>
+  </si>
+  <si>
+    <t>Lagged operational gap index (t−1)</t>
+  </si>
+  <si>
+    <t>Lagged peer pressure index (t−1)</t>
+  </si>
+  <si>
+    <t>Lagged bonus eligibility flag (t−1)</t>
+  </si>
+  <si>
+    <t>lag_decision_latency_avg</t>
+  </si>
+  <si>
+    <t>Lagged decision latency (t−1)</t>
+  </si>
+  <si>
+    <t>Optional; include only if used</t>
+  </si>
+  <si>
+    <t>panel_manager_period_outcomes</t>
+  </si>
+  <si>
+    <t>Manager identifier</t>
+  </si>
+  <si>
+    <t>3-week period identifier</t>
+  </si>
+  <si>
+    <t>FK → panel_manager_period</t>
+  </si>
+  <si>
+    <t>service_level_pct</t>
+  </si>
+  <si>
+    <t>Realized service level in period</t>
+  </si>
+  <si>
+    <t>POST_HMM_OUTCOME</t>
+  </si>
+  <si>
+    <t>Used for validation / consequence analysis</t>
+  </si>
+  <si>
+    <t>inventory_cost_eur</t>
+  </si>
+  <si>
+    <t>Realized inventory holding cost</t>
+  </si>
+  <si>
+    <t>expedite_cost_eur</t>
+  </si>
+  <si>
+    <t>Realized expediting / emergency logistics cost</t>
+  </si>
+  <si>
+    <t>Count of major operational incidents/errors</t>
+  </si>
+  <si>
+    <t>Must not be used for state identification</t>
+  </si>
+  <si>
+    <t>production_disruption_minutes</t>
+  </si>
+  <si>
+    <t>Minutes of production disruption/stoppage</t>
+  </si>
+  <si>
+    <t>L1 panel (employee-period)</t>
+  </si>
+  <si>
+    <t>Aligns with manager panel</t>
+  </si>
+  <si>
+    <t>Site/plant context for employee</t>
+  </si>
+  <si>
+    <t>Share of tasks executed autonomously by AI</t>
+  </si>
+  <si>
+    <t>Real authority measure</t>
+  </si>
+  <si>
+    <t>Complement of AI share</t>
+  </si>
+  <si>
+    <t>Collaboration indicator</t>
+  </si>
+  <si>
+    <t>Fraction of tasks requiring rework/correction</t>
+  </si>
+  <si>
+    <t>Fraction of tasks with execution errors</t>
+  </si>
+  <si>
+    <t>Useful as normalization / control in post-HMM models</t>
+  </si>
+  <si>
+    <t>Coordination/interdependence complexity of tasks</t>
+  </si>
+  <si>
+    <t>Control in post-HMM models</t>
+  </si>
+  <si>
+    <t>Degree of AI assistance used by employee</t>
+  </si>
+  <si>
+    <t>Unique decision episode identifier</t>
+  </si>
+  <si>
+    <t>Used for aggregation to panel_manager_period</t>
+  </si>
+  <si>
+    <t>Type/class of recommendation</t>
+  </si>
+  <si>
+    <t>AGGREGATION_SOURCE</t>
+  </si>
+  <si>
+    <t>Optional stratification</t>
+  </si>
+  <si>
+    <t>AI confidence score</t>
+  </si>
+  <si>
+    <t>ROBUSTNESS_ONLY</t>
+  </si>
+  <si>
+    <t>Optional: acceptance/override moderation</t>
+  </si>
+  <si>
+    <t>Optional: escalation/override mechanism</t>
+  </si>
+  <si>
+    <t>Explanation shown/available in episode</t>
+  </si>
+  <si>
+    <t>Proxy for episode-level transparency</t>
+  </si>
+  <si>
+    <t>Manager action category (accept/partial/reject)</t>
+  </si>
+  <si>
+    <t>Source for alternative rate measures</t>
+  </si>
+  <si>
+    <t>override_pct</t>
+  </si>
+  <si>
+    <t>Override magnitude in episode</t>
+  </si>
+  <si>
+    <t>Aggregates to mean_override_pct</t>
+  </si>
+  <si>
+    <t>Time from recommendation to manager decision</t>
+  </si>
+  <si>
+    <t>Aggregates to decision_latency_avg</t>
+  </si>
+  <si>
+    <t>Unique execution act identifier</t>
+  </si>
+  <si>
+    <t>Decision episode linked to execution</t>
+  </si>
+  <si>
+    <t>Intensity of AI assistance during execution</t>
+  </si>
+  <si>
+    <t>Aggregates to ai_support_intensity</t>
+  </si>
+  <si>
+    <t>Micro-intervention indicator</t>
+  </si>
+  <si>
+    <t>Employee made local adjustments during execution</t>
+  </si>
+  <si>
+    <t>Tacit adaptation</t>
+  </si>
+  <si>
+    <t>Aggregates to avg_execution_time</t>
+  </si>
+  <si>
+    <t>Aggregates to error_rate</t>
+  </si>
+  <si>
+    <t>Manager role title</t>
+  </si>
+  <si>
+    <t>Stable / slow-moving</t>
+  </si>
+  <si>
+    <t>Functional area</t>
+  </si>
+  <si>
+    <t>Years of managerial seniority</t>
+  </si>
+  <si>
+    <t>Heterogeneity / moderation</t>
+  </si>
+  <si>
+    <t>Used for heterogeneity; π is uniform in main model</t>
+  </si>
+  <si>
+    <t>Employee role</t>
+  </si>
+  <si>
+    <t>Familiarity with AI tools</t>
+  </si>
+  <si>
+    <t>Heterogeneity</t>
+  </si>
+  <si>
+    <t>Deployment date of AI version</t>
+  </si>
+  <si>
+    <t>Used to compute implementation age if needed</t>
+  </si>
+  <si>
+    <t>Degree of autonomy</t>
+  </si>
+  <si>
+    <t>Governance design lever</t>
+  </si>
+  <si>
+    <t>Explanation capability level</t>
+  </si>
+  <si>
+    <t>Transparency design lever</t>
+  </si>
+  <si>
+    <t>Calibration quality of AI confidence</t>
+  </si>
+  <si>
+    <t>Signal quality indicator</t>
+  </si>
+  <si>
+    <t>Unique site identifier</t>
+  </si>
+  <si>
+    <t>Site type</t>
+  </si>
+  <si>
+    <t>Site automation maturity</t>
+  </si>
+  <si>
+    <t>Context / moderation</t>
+  </si>
+  <si>
+    <t>Structural operational complexity</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">The dataset used in this study consists of longitudinal field data collected from a large German original equipment manufacturer (OEM) operating an </t>
+      <t xml:space="preserve">The dataset used in this study consists of longitudinal field data collected from a large German original equipment manufacturer (OEM) operating an AI-enabled inventory reallocation system. The empirical setting spans multi-plant production and logistics operations, where persistent inventory imbalances across plants can trigger costly stockouts, excess holding costs, and even production line stoppages. To mitigate these risks, the firm has integrated an AI-based decision support system into its enterprise resource planning (ERP) and supply-chain planning infrastructure. The system continuously generates reallocation recommendations across plants, embedding AI into managers’ day-to-day operational decision processes and creating a rich context to observe how managerial delegation to AI unfolds over time.
+The study analyzes delegation dynamics using a multi-level longitudinal dataset spanning approximately </t>
     </r>
     <r>
       <rPr>
@@ -652,7 +1208,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>AI-enabled inventory reallocation system</t>
+      <t xml:space="preserve">1.5 years, </t>
     </r>
     <r>
       <rPr>
@@ -661,8 +1217,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">. The empirical setting spans multi-plant production and logistics operations, where persistent inventory imbalances across plants can trigger costly stockouts, excess holding costs, and even production line stoppages. To mitigate these risks, the firm has integrated an AI-based decision support system into its enterprise resource planning (ERP) and supply-chain planning infrastructure. The system continuously generates reallocation recommendations across plants, embedding AI into managers’ day-to-day operational decision processes and creating a rich context to observe how managerial delegation to AI unfolds over time.
-The study analyzes AI delegation dynamics at a multinational manufacturer using a multi‑level dataset spanning </t>
+      <t xml:space="preserve">structured around repeated three-week decision cycles corresponding to the firm’s planning and reallocation cadence. The dataset includes </t>
     </r>
     <r>
       <rPr>
@@ -672,7 +1227,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>1.5 years.</t>
+      <t>120 operations managers across 12 manufacturing sites, observed over 26 decision periods, yielding 3,120 manager-period observations in the core panel. In addition</t>
     </r>
     <r>
       <rPr>
@@ -681,7 +1236,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> It includes </t>
+      <t xml:space="preserve">, the dataset contains execution-side records for </t>
     </r>
     <r>
       <rPr>
@@ -691,7 +1246,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>2,847 managers across 29 sites observed over 26 decision periods</t>
+      <t>680 specialized employees,</t>
     </r>
     <r>
       <rPr>
@@ -700,7 +1255,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">, plus execution records for </t>
+      <t xml:space="preserve"> captured in an employee-period panel with </t>
     </r>
     <r>
       <rPr>
@@ -710,7 +1265,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>1,334 specialized employees</t>
+      <t>17,680 observations,</t>
     </r>
     <r>
       <rPr>
@@ -719,563 +1274,8 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> who carry out tasks either autonomously, with AI support, or manually. This longitudinal panel captures variations in delegation authority, execution responsibility, and coordination, providing scale and temporal depth suited for dynamic modeling.</t>
+      <t xml:space="preserve"> reflecting whether tasks are executed manually, with AI support, or in more automated modes. Together, these linked panels capture systematic variation in decision authority (delegation shares, override and escalation behavior), execution responsibility (employee-side AI support intensity), and coordination outcomes (decision latency and performance deltas), providing scale and temporal depth suited for dynamic modeling of latent delegation regimes.</t>
     </r>
-  </si>
-  <si>
-    <t>II. Data Structure</t>
-  </si>
-  <si>
-    <t>├── LEVEL 1 — Dynamic Panels (HMM Estimation &amp; Outcomes)</t>
-  </si>
-  <si>
-    <t>│   ├── panel_manager_period   [PRIMARY HMM ESTIMATION TABLE]</t>
-  </si>
-  <si>
-    <t>│   │      Purpose: Formal decision authority delegation &amp; learning dynamics</t>
-  </si>
-  <si>
-    <t>│   │   ├── Identifiers &amp; time index</t>
-  </si>
-  <si>
-    <t>│   │   │   ├── period_start_date</t>
-  </si>
-  <si>
-    <t>│   │   │   ├── period_end_date</t>
-  </si>
-  <si>
-    <t>│   │   │   ├── weeks_in_period</t>
-  </si>
-  <si>
-    <t>│   │   ├── Formal decision authority (HMM emissions)</t>
-  </si>
-  <si>
-    <t>│   │   │   ├── ai_decision_authority_share        [EMISSION 1]</t>
-  </si>
-  <si>
-    <t>│   │   │   └── mean_override_pct                   [EMISSION 2]</t>
-  </si>
-  <si>
-    <t>│   │   ├── Performance feedback (HMM transition drivers)</t>
-  </si>
-  <si>
-    <t>│   │   │   ├── kpi_operational_gap_index</t>
-  </si>
-  <si>
-    <t>│   │   │   ├── kpi_peer_pressure_index</t>
-  </si>
-  <si>
-    <t>│   │   │   └── bonus_eligibility_flag              [SALIENT SHOCK]</t>
-  </si>
-  <si>
-    <t>│   │   ├── Incentives &amp; governance context (controls / moderators)</t>
-  </si>
-  <si>
-    <t>│   │   ├── Environmental &amp; task context (controls)</t>
-  </si>
-  <si>
-    <t>│   │   │   ├── task_complexity_index</t>
-  </si>
-  <si>
-    <t>│   │   │   ├── supply_disruption_count</t>
-  </si>
-  <si>
-    <t>│   │   │   └── forecast_accuracy_mape</t>
-  </si>
-  <si>
-    <t>│   │   └── Derived lag variables (explicit)</t>
-  </si>
-  <si>
-    <t>│   │       ├── lag_ai_decision_authority_share</t>
-  </si>
-  <si>
-    <t>│   │       ├── lag_mean_override_pct</t>
-  </si>
-  <si>
-    <t>│   │       ├── lag_kpi_operational_gap_index</t>
-  </si>
-  <si>
-    <t>│   │       ├── lag_kpi_peer_pressure_index</t>
-  </si>
-  <si>
-    <t>│   │       ├── lag_bonus_eligibility_flag</t>
-  </si>
-  <si>
-    <t>│   │       └── lag_decision_latency_avg   (optional)</t>
-  </si>
-  <si>
-    <t>│   ├── panel_manager_period_outcomes   [POST-HMM VALIDATION / CONSEQUENCES]</t>
-  </si>
-  <si>
-    <t>│   │      Actor: Manager / Site</t>
-  </si>
-  <si>
-    <t>│   │      Purpose: Operational outcomes (not used for state identification)</t>
-  </si>
-  <si>
-    <t>│   │   ├── service_level_pct</t>
-  </si>
-  <si>
-    <t>│   │   ├── inventory_cost_eur</t>
-  </si>
-  <si>
-    <t>│   │   ├── expedite_cost_eur</t>
-  </si>
-  <si>
-    <t>│   │   ├── error_incident_count</t>
-  </si>
-  <si>
-    <t>│   │   └── production_disruption_minutes</t>
-  </si>
-  <si>
-    <t>│   └── panel_employee_period   [REAL AUTHORITY / EXECUTION PANEL]</t>
-  </si>
-  <si>
-    <t>│          Purpose: Execution responsibility &amp; coordination with AI</t>
-  </si>
-  <si>
-    <t>│       ├── Execution responsibility (real authority)</t>
-  </si>
-  <si>
-    <t>├── LEVEL 2 — Episode Data (Behavioral Micro-Foundations)</t>
-  </si>
-  <si>
-    <t>│   ├── decision_episode   [MANAGER ↔ AI MICRO-DECISIONS]</t>
-  </si>
-  <si>
-    <t>│   │      Purpose: Micro-level inputs aggregated into HMM emissions &amp; controls</t>
-  </si>
-  <si>
-    <t>│   │       ├── manager_action            (accept / partial / reject)</t>
-  </si>
-  <si>
-    <t>│   │       ├── override_pct              → mean_override_pct</t>
-  </si>
-  <si>
-    <t>│   │       └── time_to_decision           → decision_latency_avg</t>
-  </si>
-  <si>
-    <t>│   └── execution_episode   [EMPLOYEE ↔ AI MICRO-EXECUTION]</t>
-  </si>
-  <si>
-    <t>│          Purpose: Micro-level execution &amp; intervention behavior</t>
-  </si>
-  <si>
-    <t>└── LEVEL 3 — Master Data (Stable Attributes &amp; Context)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ├── manager_master   [HETEROGENEITY / MODERATION]</t>
-  </si>
-  <si>
-    <t>│   │   │   ├── kpi_industry_gap_index</t>
-  </si>
-  <si>
-    <t>period_start_date</t>
-  </si>
-  <si>
-    <t>Used for lag construction</t>
-  </si>
-  <si>
-    <t>period_end_date</t>
-  </si>
-  <si>
-    <t>—</t>
-  </si>
-  <si>
-    <t>weeks_in_period</t>
-  </si>
-  <si>
-    <t>Length of period</t>
-  </si>
-  <si>
-    <t>weeks</t>
-  </si>
-  <si>
-    <t>mean_override_pct</t>
-  </si>
-  <si>
-    <t>Average magnitude of manager overrides of AI recommendations</t>
-  </si>
-  <si>
-    <t>kpi_operational_gap_index</t>
-  </si>
-  <si>
-    <t>Composite index of within-team KPI change vs prior period</t>
-  </si>
-  <si>
-    <t>standardized index</t>
-  </si>
-  <si>
-    <t>kpi_peer_pressure_index</t>
-  </si>
-  <si>
-    <t>Composite index of KPI standing relative to peer teams</t>
-  </si>
-  <si>
-    <t>bonus_eligibility_flag</t>
-  </si>
-  <si>
-    <t>Salient incentive discontinuity</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>lag_ai_decision_authority_share</t>
-  </si>
-  <si>
-    <t>lag_mean_override_pct</t>
-  </si>
-  <si>
-    <t>lag_kpi_operational_gap_index</t>
-  </si>
-  <si>
-    <t>lag_kpi_peer_pressure_index</t>
-  </si>
-  <si>
-    <t>lag_bonus_eligibility_flag</t>
-  </si>
-  <si>
-    <t>IDENTIFIER</t>
-  </si>
-  <si>
-    <t>HMM_EMISSION</t>
-  </si>
-  <si>
-    <t>HMM_TRANSITION_DRIVER</t>
-  </si>
-  <si>
-    <t>HMM_TRANSITION_SHOCK</t>
-  </si>
-  <si>
-    <t>HMM_CONTROL</t>
-  </si>
-  <si>
-    <t>HMM_LAG</t>
-  </si>
-  <si>
-    <t>L1 panel (manager-period)</t>
-  </si>
-  <si>
-    <t>3-week decision period identifier</t>
-  </si>
-  <si>
-    <t>Shared across panel tables</t>
-  </si>
-  <si>
-    <t>Start date of the decision period</t>
-  </si>
-  <si>
-    <t>End date of the decision period</t>
-  </si>
-  <si>
-    <t>Typically 3</t>
-  </si>
-  <si>
-    <t>AI system version active during period</t>
-  </si>
-  <si>
-    <t>CONTEXT_MASTER</t>
-  </si>
-  <si>
-    <t>Share of decisions where manager delegates formal decision authority to AI</t>
-  </si>
-  <si>
-    <t>Primary state-identifying behavioral measure</t>
-  </si>
-  <si>
-    <t>Derived from decision_episode.override_pct</t>
-  </si>
-  <si>
-    <t>Reduced-form performance feedback signal</t>
-  </si>
-  <si>
-    <t>Captures peer comparison / relative pressure</t>
-  </si>
-  <si>
-    <t>Indicator that period performance affects bonus eligibility</t>
-  </si>
-  <si>
-    <t>Difficulty/tightness of targets assigned in period</t>
-  </si>
-  <si>
-    <t>Governance context; exogenous where possible</t>
-  </si>
-  <si>
-    <t>Emission/transition control (context difficulty)</t>
-  </si>
-  <si>
-    <t>Number of supply disruptions affecting manager scope in period</t>
-  </si>
-  <si>
-    <t>Exogenous operational turbulence</t>
-  </si>
-  <si>
-    <t>Forecast error (MAPE) for manager scope during period</t>
-  </si>
-  <si>
-    <t>Proxy for signal quality; lower is better</t>
-  </si>
-  <si>
-    <t>Lagged AI decision authority share (t−1)</t>
-  </si>
-  <si>
-    <t>Derived from prior period</t>
-  </si>
-  <si>
-    <t>Lagged override magnitude (t−1)</t>
-  </si>
-  <si>
-    <t>Lagged operational gap index (t−1)</t>
-  </si>
-  <si>
-    <t>Lagged peer pressure index (t−1)</t>
-  </si>
-  <si>
-    <t>Lagged bonus eligibility flag (t−1)</t>
-  </si>
-  <si>
-    <t>lag_decision_latency_avg</t>
-  </si>
-  <si>
-    <t>Lagged decision latency (t−1)</t>
-  </si>
-  <si>
-    <t>Optional; include only if used</t>
-  </si>
-  <si>
-    <t>panel_manager_period_outcomes</t>
-  </si>
-  <si>
-    <t>Manager identifier</t>
-  </si>
-  <si>
-    <t>3-week period identifier</t>
-  </si>
-  <si>
-    <t>FK → panel_manager_period</t>
-  </si>
-  <si>
-    <t>service_level_pct</t>
-  </si>
-  <si>
-    <t>Realized service level in period</t>
-  </si>
-  <si>
-    <t>POST_HMM_OUTCOME</t>
-  </si>
-  <si>
-    <t>Used for validation / consequence analysis</t>
-  </si>
-  <si>
-    <t>inventory_cost_eur</t>
-  </si>
-  <si>
-    <t>Realized inventory holding cost</t>
-  </si>
-  <si>
-    <t>expedite_cost_eur</t>
-  </si>
-  <si>
-    <t>Realized expediting / emergency logistics cost</t>
-  </si>
-  <si>
-    <t>Count of major operational incidents/errors</t>
-  </si>
-  <si>
-    <t>Must not be used for state identification</t>
-  </si>
-  <si>
-    <t>production_disruption_minutes</t>
-  </si>
-  <si>
-    <t>Minutes of production disruption/stoppage</t>
-  </si>
-  <si>
-    <t>L1 panel (employee-period)</t>
-  </si>
-  <si>
-    <t>Aligns with manager panel</t>
-  </si>
-  <si>
-    <t>Site/plant context for employee</t>
-  </si>
-  <si>
-    <t>Share of tasks executed autonomously by AI</t>
-  </si>
-  <si>
-    <t>Real authority measure</t>
-  </si>
-  <si>
-    <t>Complement of AI share</t>
-  </si>
-  <si>
-    <t>Collaboration indicator</t>
-  </si>
-  <si>
-    <t>Fraction of tasks requiring rework/correction</t>
-  </si>
-  <si>
-    <t>Fraction of tasks with execution errors</t>
-  </si>
-  <si>
-    <t>Useful as normalization / control in post-HMM models</t>
-  </si>
-  <si>
-    <t>Coordination/interdependence complexity of tasks</t>
-  </si>
-  <si>
-    <t>Control in post-HMM models</t>
-  </si>
-  <si>
-    <t>Degree of AI assistance used by employee</t>
-  </si>
-  <si>
-    <t>Unique decision episode identifier</t>
-  </si>
-  <si>
-    <t>Used for aggregation to panel_manager_period</t>
-  </si>
-  <si>
-    <t>Type/class of recommendation</t>
-  </si>
-  <si>
-    <t>AGGREGATION_SOURCE</t>
-  </si>
-  <si>
-    <t>Optional stratification</t>
-  </si>
-  <si>
-    <t>AI confidence score</t>
-  </si>
-  <si>
-    <t>ROBUSTNESS_ONLY</t>
-  </si>
-  <si>
-    <t>Optional: acceptance/override moderation</t>
-  </si>
-  <si>
-    <t>Optional: escalation/override mechanism</t>
-  </si>
-  <si>
-    <t>Explanation shown/available in episode</t>
-  </si>
-  <si>
-    <t>Proxy for episode-level transparency</t>
-  </si>
-  <si>
-    <t>Manager action category (accept/partial/reject)</t>
-  </si>
-  <si>
-    <t>Source for alternative rate measures</t>
-  </si>
-  <si>
-    <t>override_pct</t>
-  </si>
-  <si>
-    <t>Override magnitude in episode</t>
-  </si>
-  <si>
-    <t>Aggregates to mean_override_pct</t>
-  </si>
-  <si>
-    <t>Time from recommendation to manager decision</t>
-  </si>
-  <si>
-    <t>Aggregates to decision_latency_avg</t>
-  </si>
-  <si>
-    <t>Unique execution act identifier</t>
-  </si>
-  <si>
-    <t>Decision episode linked to execution</t>
-  </si>
-  <si>
-    <t>Intensity of AI assistance during execution</t>
-  </si>
-  <si>
-    <t>Aggregates to ai_support_intensity</t>
-  </si>
-  <si>
-    <t>Micro-intervention indicator</t>
-  </si>
-  <si>
-    <t>Employee made local adjustments during execution</t>
-  </si>
-  <si>
-    <t>Tacit adaptation</t>
-  </si>
-  <si>
-    <t>Aggregates to avg_execution_time</t>
-  </si>
-  <si>
-    <t>Aggregates to error_rate</t>
-  </si>
-  <si>
-    <t>Manager role title</t>
-  </si>
-  <si>
-    <t>Stable / slow-moving</t>
-  </si>
-  <si>
-    <t>Functional area</t>
-  </si>
-  <si>
-    <t>Years of managerial seniority</t>
-  </si>
-  <si>
-    <t>Heterogeneity / moderation</t>
-  </si>
-  <si>
-    <t>Used for heterogeneity; π is uniform in main model</t>
-  </si>
-  <si>
-    <t>Employee role</t>
-  </si>
-  <si>
-    <t>Familiarity with AI tools</t>
-  </si>
-  <si>
-    <t>Heterogeneity</t>
-  </si>
-  <si>
-    <t>Deployment date of AI version</t>
-  </si>
-  <si>
-    <t>Used to compute implementation age if needed</t>
-  </si>
-  <si>
-    <t>Degree of autonomy</t>
-  </si>
-  <si>
-    <t>Governance design lever</t>
-  </si>
-  <si>
-    <t>Explanation capability level</t>
-  </si>
-  <si>
-    <t>Transparency design lever</t>
-  </si>
-  <si>
-    <t>Calibration quality of AI confidence</t>
-  </si>
-  <si>
-    <t>Signal quality indicator</t>
-  </si>
-  <si>
-    <t>Unique site identifier</t>
-  </si>
-  <si>
-    <t>Site type</t>
-  </si>
-  <si>
-    <t>Site automation maturity</t>
-  </si>
-  <si>
-    <t>Context / moderation</t>
-  </si>
-  <si>
-    <t>Structural operational complexity</t>
   </si>
 </sst>
 </file>
@@ -1943,8 +1943,8 @@
   </sheetPr>
   <dimension ref="A1:J242"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G143" sqref="G143"/>
+    <sheetView tabSelected="1" topLeftCell="A95" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1957,9 +1957,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="227.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="289.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="25" t="s">
-        <v>206</v>
+        <v>391</v>
       </c>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
@@ -1973,7 +1973,7 @@
     </row>
     <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="31.8" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -2032,7 +2032,7 @@
     </row>
     <row r="9" spans="1:10" s="4" customFormat="1" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -2060,7 +2060,7 @@
     </row>
     <row r="11" spans="1:10" s="21" customFormat="1" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
@@ -2102,7 +2102,7 @@
     </row>
     <row r="14" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -2130,7 +2130,7 @@
     </row>
     <row r="16" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -2172,7 +2172,7 @@
     </row>
     <row r="19" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
@@ -2186,7 +2186,7 @@
     </row>
     <row r="20" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
@@ -2200,7 +2200,7 @@
     </row>
     <row r="21" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B21" s="11"/>
       <c r="C21" s="11"/>
@@ -2242,7 +2242,7 @@
     </row>
     <row r="24" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="11"/>
@@ -2256,7 +2256,7 @@
     </row>
     <row r="25" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="13" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
@@ -2270,7 +2270,7 @@
     </row>
     <row r="26" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B26" s="11"/>
       <c r="C26" s="11"/>
@@ -2298,7 +2298,7 @@
     </row>
     <row r="28" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B28" s="11"/>
       <c r="C28" s="11"/>
@@ -2312,7 +2312,7 @@
     </row>
     <row r="29" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -2326,7 +2326,7 @@
     </row>
     <row r="30" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="11"/>
@@ -2340,7 +2340,7 @@
     </row>
     <row r="31" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -2354,7 +2354,7 @@
     </row>
     <row r="32" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B32" s="11"/>
       <c r="C32" s="11"/>
@@ -2382,7 +2382,7 @@
     </row>
     <row r="34" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
@@ -2438,7 +2438,7 @@
     </row>
     <row r="38" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
@@ -2452,7 +2452,7 @@
     </row>
     <row r="39" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B39" s="11"/>
       <c r="C39" s="11"/>
@@ -2466,7 +2466,7 @@
     </row>
     <row r="40" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B40" s="11"/>
       <c r="C40" s="11"/>
@@ -2480,7 +2480,7 @@
     </row>
     <row r="41" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="11"/>
@@ -2508,7 +2508,7 @@
     </row>
     <row r="43" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B43" s="11"/>
       <c r="C43" s="11"/>
@@ -2522,7 +2522,7 @@
     </row>
     <row r="44" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B44" s="11"/>
       <c r="C44" s="11"/>
@@ -2536,7 +2536,7 @@
     </row>
     <row r="45" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
@@ -2550,7 +2550,7 @@
     </row>
     <row r="46" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B46" s="11"/>
       <c r="C46" s="11"/>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="47" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -2578,7 +2578,7 @@
     </row>
     <row r="48" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B48" s="11"/>
       <c r="C48" s="11"/>
@@ -2592,7 +2592,7 @@
     </row>
     <row r="49" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B49" s="11"/>
       <c r="C49" s="11"/>
@@ -2620,7 +2620,7 @@
     </row>
     <row r="51" spans="1:10" s="21" customFormat="1" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B51" s="20"/>
       <c r="C51" s="20"/>
@@ -2634,7 +2634,7 @@
     </row>
     <row r="52" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B52" s="11"/>
       <c r="C52" s="11"/>
@@ -2662,7 +2662,7 @@
     </row>
     <row r="54" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B54" s="11"/>
       <c r="C54" s="11"/>
@@ -2690,7 +2690,7 @@
     </row>
     <row r="56" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B56" s="11"/>
       <c r="C56" s="11"/>
@@ -2704,7 +2704,7 @@
     </row>
     <row r="57" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B57" s="11"/>
       <c r="C57" s="11"/>
@@ -2718,7 +2718,7 @@
     </row>
     <row r="58" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B58" s="11"/>
       <c r="C58" s="11"/>
@@ -2732,7 +2732,7 @@
     </row>
     <row r="59" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B59" s="11"/>
       <c r="C59" s="11"/>
@@ -2746,7 +2746,7 @@
     </row>
     <row r="60" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B60" s="11"/>
       <c r="C60" s="11"/>
@@ -2774,7 +2774,7 @@
     </row>
     <row r="62" spans="1:10" s="21" customFormat="1" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="19" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B62" s="20"/>
       <c r="C62" s="20"/>
@@ -2816,7 +2816,7 @@
     </row>
     <row r="65" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B65" s="11"/>
       <c r="C65" s="11"/>
@@ -2928,7 +2928,7 @@
     </row>
     <row r="73" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B73" s="11"/>
       <c r="C73" s="11"/>
@@ -3138,7 +3138,7 @@
     </row>
     <row r="88" spans="1:10" s="4" customFormat="1" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B88" s="12"/>
       <c r="C88" s="12"/>
@@ -3166,7 +3166,7 @@
     </row>
     <row r="90" spans="1:10" s="21" customFormat="1" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B90" s="20"/>
       <c r="C90" s="20"/>
@@ -3194,7 +3194,7 @@
     </row>
     <row r="92" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B92" s="11"/>
       <c r="C92" s="11"/>
@@ -3418,7 +3418,7 @@
     </row>
     <row r="108" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B108" s="11"/>
       <c r="C108" s="11"/>
@@ -3432,7 +3432,7 @@
     </row>
     <row r="109" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B109" s="11"/>
       <c r="C109" s="11"/>
@@ -3446,7 +3446,7 @@
     </row>
     <row r="110" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B110" s="11"/>
       <c r="C110" s="11"/>
@@ -3474,7 +3474,7 @@
     </row>
     <row r="112" spans="1:10" s="21" customFormat="1" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B112" s="20"/>
       <c r="C112" s="20"/>
@@ -3502,7 +3502,7 @@
     </row>
     <row r="114" spans="1:10" ht="15.3" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B114" s="11"/>
       <c r="C114" s="11"/>
@@ -3782,7 +3782,7 @@
     </row>
     <row r="134" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B134" s="12"/>
       <c r="C134" s="12"/>
@@ -3810,7 +3810,7 @@
     </row>
     <row r="136" spans="1:10" s="21" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B136" s="20"/>
       <c r="C136" s="20"/>
@@ -5164,7 +5164,7 @@
   </sheetPr>
   <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A66" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
@@ -5218,10 +5218,10 @@
         <v>104</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G2" s="24" t="s">
         <v>105</v>
@@ -5235,19 +5235,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D3" s="24" t="s">
         <v>106</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.5">
@@ -5255,22 +5255,22 @@
         <v>19</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D4" s="24" t="s">
         <v>24</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.5">
@@ -5278,22 +5278,22 @@
         <v>19</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.5">
@@ -5301,22 +5301,22 @@
         <v>19</v>
       </c>
       <c r="B6" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>260</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="D6" s="24" t="s">
         <v>261</v>
       </c>
-      <c r="D6" s="24" t="s">
-        <v>262</v>
-      </c>
       <c r="E6" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G6" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.5">
@@ -5327,16 +5327,16 @@
         <v>6</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G7" s="24" t="s">
         <v>119</v>
@@ -5350,19 +5350,19 @@
         <v>2</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>107</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="28.2" x14ac:dyDescent="0.5">
@@ -5370,22 +5370,22 @@
         <v>19</v>
       </c>
       <c r="B9" s="24" t="s">
+        <v>262</v>
+      </c>
+      <c r="C9" s="24" t="s">
         <v>263</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>264</v>
       </c>
       <c r="D9" s="24" t="s">
         <v>107</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G9" s="24" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28.2" x14ac:dyDescent="0.5">
@@ -5393,22 +5393,22 @@
         <v>19</v>
       </c>
       <c r="B10" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="C10" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="D10" s="24" t="s">
         <v>266</v>
       </c>
-      <c r="D10" s="24" t="s">
-        <v>267</v>
-      </c>
       <c r="E10" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G10" s="24" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="28.2" x14ac:dyDescent="0.5">
@@ -5416,22 +5416,22 @@
         <v>19</v>
       </c>
       <c r="B11" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="C11" s="24" t="s">
         <v>268</v>
       </c>
-      <c r="C11" s="24" t="s">
-        <v>269</v>
-      </c>
       <c r="D11" s="24" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G11" s="24" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="28.2" x14ac:dyDescent="0.5">
@@ -5439,22 +5439,22 @@
         <v>19</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D12" s="24" t="s">
         <v>116</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G12" s="24" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.5">
@@ -5465,19 +5465,19 @@
         <v>114</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>115</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="28.2" x14ac:dyDescent="0.5">
@@ -5494,10 +5494,10 @@
         <v>110</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G14" s="24" t="s">
         <v>111</v>
@@ -5517,13 +5517,13 @@
         <v>23</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G15" s="24" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="28.2" x14ac:dyDescent="0.5">
@@ -5534,19 +5534,19 @@
         <v>5</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D16" s="24" t="s">
         <v>21</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="28.2" x14ac:dyDescent="0.5">
@@ -5557,19 +5557,19 @@
         <v>4</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D17" s="24" t="s">
         <v>118</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.5">
@@ -5577,22 +5577,22 @@
         <v>19</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>155</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.5">
@@ -5600,22 +5600,22 @@
         <v>19</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D19" s="24" t="s">
         <v>155</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.5">
@@ -5623,22 +5623,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D20" s="24" t="s">
         <v>23</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.5">
@@ -5646,22 +5646,22 @@
         <v>19</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D21" s="24" t="s">
         <v>23</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.5">
@@ -5669,22 +5669,22 @@
         <v>19</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D22" s="24" t="s">
         <v>116</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.5">
@@ -5692,42 +5692,42 @@
         <v>19</v>
       </c>
       <c r="B23" s="24" t="s">
+        <v>310</v>
+      </c>
+      <c r="C23" s="24" t="s">
         <v>311</v>
-      </c>
-      <c r="C23" s="24" t="s">
-        <v>312</v>
       </c>
       <c r="D23" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A24" s="24" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B24" s="24" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D24" s="24" t="s">
         <v>104</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G24" s="24" t="s">
         <v>105</v>
@@ -5735,140 +5735,140 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A25" s="24" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B25" s="24" t="s">
         <v>1</v>
       </c>
       <c r="C25" s="24" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D25" s="24" t="s">
         <v>106</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A26" s="24" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B26" s="24" t="s">
+        <v>317</v>
+      </c>
+      <c r="C26" s="24" t="s">
         <v>318</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="D26" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="E26" s="24" t="s">
+        <v>283</v>
+      </c>
+      <c r="F26" s="24" t="s">
         <v>319</v>
       </c>
-      <c r="D26" s="24" t="s">
-        <v>272</v>
-      </c>
-      <c r="E26" s="24" t="s">
-        <v>284</v>
-      </c>
-      <c r="F26" s="24" t="s">
+      <c r="G26" s="24" t="s">
         <v>320</v>
-      </c>
-      <c r="G26" s="24" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A27" s="24" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B27" s="24" t="s">
+        <v>321</v>
+      </c>
+      <c r="C27" s="24" t="s">
         <v>322</v>
-      </c>
-      <c r="C27" s="24" t="s">
-        <v>323</v>
       </c>
       <c r="D27" s="24" t="s">
         <v>112</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F27" s="24" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A28" s="24" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B28" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="C28" s="24" t="s">
         <v>324</v>
-      </c>
-      <c r="C28" s="24" t="s">
-        <v>325</v>
       </c>
       <c r="D28" s="24" t="s">
         <v>112</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G28" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A29" s="24" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B29" s="24" t="s">
         <v>113</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D29" s="24" t="s">
         <v>21</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G29" s="24" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A30" s="24" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B30" s="24" t="s">
+        <v>327</v>
+      </c>
+      <c r="C30" s="24" t="s">
         <v>328</v>
-      </c>
-      <c r="C30" s="24" t="s">
-        <v>329</v>
       </c>
       <c r="D30" s="24" t="s">
         <v>22</v>
       </c>
       <c r="E30" s="24" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F30" s="24" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G30" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.5">
@@ -5885,10 +5885,10 @@
         <v>104</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G31" s="24" t="s">
         <v>122</v>
@@ -5908,10 +5908,10 @@
         <v>104</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F32" s="24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G32" s="24" t="s">
         <v>105</v>
@@ -5925,19 +5925,19 @@
         <v>1</v>
       </c>
       <c r="C33" s="24" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D33" s="24" t="s">
         <v>106</v>
       </c>
       <c r="E33" s="24" t="s">
+        <v>329</v>
+      </c>
+      <c r="F33" s="24" t="s">
+        <v>277</v>
+      </c>
+      <c r="G33" s="24" t="s">
         <v>330</v>
-      </c>
-      <c r="F33" s="24" t="s">
-        <v>278</v>
-      </c>
-      <c r="G33" s="24" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.5">
@@ -5948,16 +5948,16 @@
         <v>124</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D34" s="24" t="s">
         <v>20</v>
       </c>
       <c r="E34" s="24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G34" s="24" t="s">
         <v>125</v>
@@ -5971,19 +5971,19 @@
         <v>126</v>
       </c>
       <c r="C35" s="24" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D35" s="24" t="s">
         <v>107</v>
       </c>
       <c r="E35" s="24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G35" s="24" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="28.2" x14ac:dyDescent="0.5">
@@ -6000,13 +6000,13 @@
         <v>107</v>
       </c>
       <c r="E36" s="24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G36" s="24" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="28.2" x14ac:dyDescent="0.5">
@@ -6023,13 +6023,13 @@
         <v>107</v>
       </c>
       <c r="E37" s="24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G37" s="24" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="28.2" x14ac:dyDescent="0.5">
@@ -6046,10 +6046,10 @@
         <v>110</v>
       </c>
       <c r="E38" s="24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G38" s="24" t="s">
         <v>133</v>
@@ -6063,16 +6063,16 @@
         <v>134</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D39" s="24" t="s">
         <v>107</v>
       </c>
       <c r="E39" s="24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F39" s="24" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G39" s="24" t="s">
         <v>135</v>
@@ -6086,16 +6086,16 @@
         <v>136</v>
       </c>
       <c r="C40" s="24" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D40" s="24" t="s">
         <v>107</v>
       </c>
       <c r="E40" s="24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F40" s="24" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G40" s="24" t="s">
         <v>137</v>
@@ -6115,13 +6115,13 @@
         <v>140</v>
       </c>
       <c r="E41" s="24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F41" s="24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G41" s="24" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.5">
@@ -6132,19 +6132,19 @@
         <v>141</v>
       </c>
       <c r="C42" s="24" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D42" s="24" t="s">
         <v>23</v>
       </c>
       <c r="E42" s="24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F42" s="24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G42" s="24" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="28.2" x14ac:dyDescent="0.5">
@@ -6155,16 +6155,16 @@
         <v>142</v>
       </c>
       <c r="C43" s="24" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D43" s="24" t="s">
         <v>143</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F43" s="24" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G43" s="24" t="s">
         <v>144</v>
@@ -6178,7 +6178,7 @@
         <v>146</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D44" s="24" t="s">
         <v>104</v>
@@ -6187,7 +6187,7 @@
         <v>147</v>
       </c>
       <c r="F44" s="24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G44" s="24" t="s">
         <v>148</v>
@@ -6210,7 +6210,7 @@
         <v>147</v>
       </c>
       <c r="F45" s="24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G45" s="24" t="s">
         <v>105</v>
@@ -6233,10 +6233,10 @@
         <v>147</v>
       </c>
       <c r="F46" s="24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G46" s="24" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.5">
@@ -6256,7 +6256,7 @@
         <v>147</v>
       </c>
       <c r="F47" s="24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G47" s="24" t="s">
         <v>125</v>
@@ -6279,7 +6279,7 @@
         <v>147</v>
       </c>
       <c r="F48" s="24" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G48" s="24" t="s">
         <v>119</v>
@@ -6293,7 +6293,7 @@
         <v>153</v>
       </c>
       <c r="C49" s="24" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D49" s="24" t="s">
         <v>20</v>
@@ -6302,10 +6302,10 @@
         <v>147</v>
       </c>
       <c r="F49" s="24" t="s">
+        <v>345</v>
+      </c>
+      <c r="G49" s="24" t="s">
         <v>346</v>
-      </c>
-      <c r="G49" s="24" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.5">
@@ -6316,7 +6316,7 @@
         <v>154</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D50" s="24" t="s">
         <v>155</v>
@@ -6325,10 +6325,10 @@
         <v>147</v>
       </c>
       <c r="F50" s="24" t="s">
+        <v>348</v>
+      </c>
+      <c r="G50" s="24" t="s">
         <v>349</v>
-      </c>
-      <c r="G50" s="24" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.5">
@@ -6348,10 +6348,10 @@
         <v>147</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G51" s="24" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.5">
@@ -6362,7 +6362,7 @@
         <v>158</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D52" s="24" t="s">
         <v>116</v>
@@ -6371,10 +6371,10 @@
         <v>147</v>
       </c>
       <c r="F52" s="24" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G52" s="24" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.5">
@@ -6385,7 +6385,7 @@
         <v>159</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D53" s="24" t="s">
         <v>20</v>
@@ -6394,10 +6394,10 @@
         <v>147</v>
       </c>
       <c r="F53" s="24" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G53" s="24" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.5">
@@ -6405,10 +6405,10 @@
         <v>145</v>
       </c>
       <c r="B54" s="24" t="s">
+        <v>355</v>
+      </c>
+      <c r="C54" s="24" t="s">
         <v>356</v>
-      </c>
-      <c r="C54" s="24" t="s">
-        <v>357</v>
       </c>
       <c r="D54" s="24" t="s">
         <v>155</v>
@@ -6417,10 +6417,10 @@
         <v>147</v>
       </c>
       <c r="F54" s="24" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G54" s="24" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.5">
@@ -6431,7 +6431,7 @@
         <v>160</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D55" s="24" t="s">
         <v>22</v>
@@ -6440,10 +6440,10 @@
         <v>147</v>
       </c>
       <c r="F55" s="24" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G55" s="24" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.5">
@@ -6454,7 +6454,7 @@
         <v>162</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D56" s="24" t="s">
         <v>104</v>
@@ -6463,7 +6463,7 @@
         <v>147</v>
       </c>
       <c r="F56" s="24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G56" s="24" t="s">
         <v>148</v>
@@ -6477,7 +6477,7 @@
         <v>146</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D57" s="24" t="s">
         <v>104</v>
@@ -6486,7 +6486,7 @@
         <v>147</v>
       </c>
       <c r="F57" s="24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G57" s="24" t="s">
         <v>163</v>
@@ -6509,7 +6509,7 @@
         <v>147</v>
       </c>
       <c r="F58" s="24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G58" s="24" t="s">
         <v>122</v>
@@ -6532,7 +6532,7 @@
         <v>147</v>
       </c>
       <c r="F59" s="24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G59" s="24" t="s">
         <v>125</v>
@@ -6555,7 +6555,7 @@
         <v>147</v>
       </c>
       <c r="F60" s="24" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G60" s="24" t="s">
         <v>168</v>
@@ -6569,7 +6569,7 @@
         <v>169</v>
       </c>
       <c r="C61" s="24" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D61" s="24" t="s">
         <v>143</v>
@@ -6578,10 +6578,10 @@
         <v>147</v>
       </c>
       <c r="F61" s="24" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G61" s="24" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="28.2" x14ac:dyDescent="0.5">
@@ -6601,10 +6601,10 @@
         <v>147</v>
       </c>
       <c r="F62" s="24" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G62" s="24" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="28.2" x14ac:dyDescent="0.5">
@@ -6615,7 +6615,7 @@
         <v>172</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D63" s="24" t="s">
         <v>116</v>
@@ -6624,10 +6624,10 @@
         <v>147</v>
       </c>
       <c r="F63" s="24" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G63" s="24" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.5">
@@ -6647,10 +6647,10 @@
         <v>147</v>
       </c>
       <c r="F64" s="24" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G64" s="24" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.5">
@@ -6670,10 +6670,10 @@
         <v>147</v>
       </c>
       <c r="F65" s="24" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G65" s="24" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.5">
@@ -6693,7 +6693,7 @@
         <v>177</v>
       </c>
       <c r="F66" s="24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G66" s="24" t="s">
         <v>148</v>
@@ -6707,7 +6707,7 @@
         <v>18</v>
       </c>
       <c r="C67" s="24" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D67" s="24" t="s">
         <v>20</v>
@@ -6716,10 +6716,10 @@
         <v>177</v>
       </c>
       <c r="F67" s="24" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G67" s="24" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.5">
@@ -6730,7 +6730,7 @@
         <v>178</v>
       </c>
       <c r="C68" s="24" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D68" s="24" t="s">
         <v>20</v>
@@ -6739,7 +6739,7 @@
         <v>177</v>
       </c>
       <c r="F68" s="24" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G68" s="24" t="s">
         <v>179</v>
@@ -6753,7 +6753,7 @@
         <v>180</v>
       </c>
       <c r="C69" s="24" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D69" s="24" t="s">
         <v>26</v>
@@ -6762,10 +6762,10 @@
         <v>177</v>
       </c>
       <c r="F69" s="24" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G69" s="24" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.5">
@@ -6785,10 +6785,10 @@
         <v>177</v>
       </c>
       <c r="F70" s="24" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G70" s="24" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.5">
@@ -6808,10 +6808,10 @@
         <v>177</v>
       </c>
       <c r="F71" s="24" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G71" s="24" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="15.3" x14ac:dyDescent="0.5">
@@ -6831,7 +6831,7 @@
         <v>177</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G72" s="6" t="s">
         <v>148</v>
@@ -6845,7 +6845,7 @@
         <v>18</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>20</v>
@@ -6854,10 +6854,10 @@
         <v>177</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="15.3" x14ac:dyDescent="0.5">
@@ -6877,10 +6877,10 @@
         <v>177</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15.3" x14ac:dyDescent="0.5">
@@ -6891,7 +6891,7 @@
         <v>190</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>183</v>
@@ -6900,10 +6900,10 @@
         <v>177</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="15.3" x14ac:dyDescent="0.5">
@@ -6923,10 +6923,10 @@
         <v>177</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="15.3" x14ac:dyDescent="0.5">
@@ -6946,7 +6946,7 @@
         <v>177</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G77" s="6" t="s">
         <v>148</v>
@@ -6960,7 +6960,7 @@
         <v>194</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>24</v>
@@ -6969,10 +6969,10 @@
         <v>177</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="15.3" x14ac:dyDescent="0.5">
@@ -6983,7 +6983,7 @@
         <v>195</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D79" s="6" t="s">
         <v>196</v>
@@ -6992,10 +6992,10 @@
         <v>177</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="15.3" x14ac:dyDescent="0.5">
@@ -7006,7 +7006,7 @@
         <v>197</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>196</v>
@@ -7015,10 +7015,10 @@
         <v>177</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="15.3" x14ac:dyDescent="0.5">
@@ -7029,7 +7029,7 @@
         <v>198</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>155</v>
@@ -7038,10 +7038,10 @@
         <v>177</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="15.3" x14ac:dyDescent="0.5">
@@ -7052,7 +7052,7 @@
         <v>124</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>20</v>
@@ -7061,7 +7061,7 @@
         <v>177</v>
       </c>
       <c r="F82" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G82" s="6" t="s">
         <v>148</v>
@@ -7084,10 +7084,10 @@
         <v>177</v>
       </c>
       <c r="F83" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="15.3" x14ac:dyDescent="0.5">
@@ -7098,7 +7098,7 @@
         <v>8</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>20</v>
@@ -7107,10 +7107,10 @@
         <v>177</v>
       </c>
       <c r="F84" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="15.3" x14ac:dyDescent="0.5">
@@ -7121,7 +7121,7 @@
         <v>202</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>203</v>
@@ -7130,10 +7130,10 @@
         <v>177</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="15.3" x14ac:dyDescent="0.5">
@@ -7144,7 +7144,7 @@
         <v>204</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>23</v>
@@ -7153,7 +7153,7 @@
         <v>177</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G86" s="6" t="s">
         <v>205</v>

</xml_diff>